<commit_message>
Ajuste escenario push notification, exclusion perfil y ejemplo AppointmentResponse e inclusion perfil y ejemplos:  Subscription, SupplyDelivery y SupplyRequest.
Ajuste escenario push notification, exclusion perfil y ejemplo AppointmentResponse e inclusion perfil y ejemplos:  Subscription, SupplyDelivery y SupplyRequest.
</commit_message>
<xml_diff>
--- a/fhir/indisa/StructureDefinition-AccountAmountKlinic.xlsx
+++ b/fhir/indisa/StructureDefinition-AccountAmountKlinic.xlsx
@@ -390,42 +390,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.03125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.34765625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.16796875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="4.58203125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.94140625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="14.70703125" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.07421875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.0625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="19.59375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="8.95703125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.4296875" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="16.2734375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="36.2890625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="37.171875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="13.86328125" customWidth="true" bestFit="true"/>
+    <col min="15" max="15" width="15.265625" customWidth="true" bestFit="true"/>
     <col min="16" max="16" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.7734375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="19.796875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="17.6015625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="40.0859375" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="15.69921875" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="13.12109375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="17.44140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="9.52734375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="17.16796875" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.65625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="21.5703125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="19.625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="42.03125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.2109375" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.4140625" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="18.18359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="10.55078125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="11.03515625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="13.87109375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="22.67578125" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="24.9765625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>